<commit_message>
updated app to save all formats
</commit_message>
<xml_diff>
--- a/data/idaho.xlsx
+++ b/data/idaho.xlsx
@@ -3682,7 +3682,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>5/29/2020</t>
+          <t>5/31/2020</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -11636,7 +11636,7 @@
       </c>
       <c r="H225" t="inlineStr">
         <is>
-          <t>5/29/2020</t>
+          <t>5/31/2020</t>
         </is>
       </c>
       <c r="I225" t="inlineStr">
@@ -14393,7 +14393,11 @@
           <t>4/30/2020</t>
         </is>
       </c>
-      <c r="I280" t="inlineStr"/>
+      <c r="I280" t="inlineStr">
+        <is>
+          <t>M,T,W,Th</t>
+        </is>
+      </c>
       <c r="J280" t="inlineStr"/>
       <c r="K280" t="inlineStr"/>
       <c r="L280" t="inlineStr"/>
@@ -14440,7 +14444,7 @@
       </c>
       <c r="H281" t="inlineStr">
         <is>
-          <t>5/29/2020</t>
+          <t>5/31/2020</t>
         </is>
       </c>
       <c r="I281" t="inlineStr">
@@ -19936,7 +19940,7 @@
       </c>
       <c r="H391" t="inlineStr">
         <is>
-          <t>5/29/2020</t>
+          <t>5/31/2020</t>
         </is>
       </c>
       <c r="I391" t="inlineStr">
@@ -20340,7 +20344,7 @@
       </c>
       <c r="H399" t="inlineStr">
         <is>
-          <t>5/29/2020</t>
+          <t>5/31/2020</t>
         </is>
       </c>
       <c r="I399" t="inlineStr">
@@ -22442,7 +22446,11 @@
           <t>3/19/2020</t>
         </is>
       </c>
-      <c r="H441" t="inlineStr"/>
+      <c r="H441" t="inlineStr">
+        <is>
+          <t>6/30/2020</t>
+        </is>
+      </c>
       <c r="I441" t="inlineStr"/>
       <c r="J441" t="inlineStr"/>
       <c r="K441" t="inlineStr"/>
@@ -26936,7 +26944,7 @@
       </c>
       <c r="H531" t="inlineStr">
         <is>
-          <t>5/29/2020</t>
+          <t>5/31/2020</t>
         </is>
       </c>
       <c r="I531" t="inlineStr">
@@ -27343,7 +27351,11 @@
           <t>4/30/2020</t>
         </is>
       </c>
-      <c r="I539" t="inlineStr"/>
+      <c r="I539" t="inlineStr">
+        <is>
+          <t>M,T,W,Th</t>
+        </is>
+      </c>
       <c r="J539" t="inlineStr"/>
       <c r="K539" t="inlineStr"/>
       <c r="L539" t="inlineStr"/>

</xml_diff>